<commit_message>
Update Check-list of the subscription form.xlsx
</commit_message>
<xml_diff>
--- a/Check-list of the subscription form.xlsx
+++ b/Check-list of the subscription form.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\404en\Documents\GitHub\Checklists\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Check-list" sheetId="1" r:id="rId4"/>
+    <sheet name="Check-list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -106,42 +114,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -149,7 +165,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -170,151 +186,55 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
-    <border/>
+  <borders count="2">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color theme="3" tint="0.59999389629810485"/>
       </left>
-    </border>
-    <border>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color theme="3" tint="0.59999389629810485"/>
       </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <top style="thin">
+        <color theme="3" tint="0.59999389629810485"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color theme="3" tint="0.59999389629810485"/>
       </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7B7B7"/>
-          <bgColor rgb="FFB7B7B7"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEFEFEF"/>
-          <bgColor rgb="FFEFEFEF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -325,18 +245,54 @@
           <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE06666"/>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -526,28 +482,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D2" sqref="D2" pane="topRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.86"/>
-    <col customWidth="1" min="2" max="2" width="119.43"/>
-    <col customWidth="1" min="3" max="3" width="26.14"/>
+    <col min="1" max="1" width="5.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="119.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="14.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,27 +518,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
@@ -587,9 +547,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>7</v>
@@ -598,9 +558,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>9</v>
@@ -609,9 +569,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>10</v>
@@ -620,9 +580,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>11</v>
@@ -631,9 +591,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>12</v>
@@ -642,9 +602,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>13</v>
@@ -653,9 +613,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>14</v>
@@ -664,9 +624,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>15</v>
@@ -675,9 +635,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>16</v>
@@ -686,9 +646,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>17</v>
@@ -697,9 +657,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>18</v>
@@ -708,9 +668,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>19</v>
@@ -719,9 +679,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>20</v>
@@ -730,9 +690,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>21</v>
@@ -741,9 +701,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>22</v>
@@ -752,9 +712,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>23</v>
@@ -763,9 +723,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>24</v>
@@ -774,9 +734,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>25</v>
@@ -785,9 +745,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>26</v>
@@ -796,9 +756,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>27</v>
@@ -807,9 +767,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>28</v>
@@ -818,25 +778,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="13">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="14" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="9" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C26">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(C4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C26">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(C4))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -846,20 +806,21 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C26">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH(("N/A"),(C4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C26">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH(("Blocked"),(C4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C26">
       <formula1>"Passed,Failed,Blocked,Skipped,N/A"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>